<commit_message>
normalised headers, added station_codes.py to be checked by other members, created To Do folder for remaining data
</commit_message>
<xml_diff>
--- a/Database/Water_quality_rivers_2018.xlsx
+++ b/Database/Water_quality_rivers_2018.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="1033">
   <si>
-    <t xml:space="preserve">Station Code</t>
+    <t xml:space="preserve">STATION CODE</t>
   </si>
   <si>
     <t xml:space="preserve">LOCATION</t>
@@ -31,52 +31,52 @@
     <t xml:space="preserve">STATE</t>
   </si>
   <si>
-    <t xml:space="preserve">Temperature (0 C) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature (0 C) max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved Oxygen (mg/ L) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved Oxygen (mg/ L) max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conductivity (µmho/ Cm) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conductivity (µmho/ Cm) max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bio- Chemical Oxygen Demand (mg/L) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bio- Chemical Oxygen Demand (mg/L) max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrate (mg/ L) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrate (mg/ L) max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faecal Coliform (MPN/ 100 mL) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faecal Coliform (MPN/ 100 mL) max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Coliform (MPN/ 100 mL) min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Coliform (MPN/ 100 mL) max</t>
+    <t xml:space="preserve">TEMPERATURE (0 C) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMPERATURE (0 C) MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISSOLVED OXYGEN (MG/ L) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISSOLVED OXYGEN (MG/ L) MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONDUCTIVITY (ΜMHO/ CM) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONDUCTIVITY (ΜMHO/ CM) MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIO- CHEMICAL OXYGEN DEMAND (MG/L) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIO- CHEMICAL OXYGEN DEMAND (MG/L) MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NITRATE (MG/ L) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NITRATE (MG/ L) MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAECAL COLIFORM (MPN/ 100 ML) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAECAL COLIFORM (MPN/ 100 ML) MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL COLIFORM (MPN/ 100 ML) MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL COLIFORM (MPN/ 100 ML) MAX</t>
   </si>
   <si>
     <t xml:space="preserve">SABARMATI AT DHAROI DAM, GUJARAT</t>
@@ -3694,15 +3694,15 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A972" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A994" activeCellId="0" sqref="A994"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="143.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.44"/>
@@ -3713,13 +3713,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="37.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="31.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="31.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="30.78"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>